<commit_message>
new plots for thesis
</commit_message>
<xml_diff>
--- a/IJR-VI/exp_results/VIpercentage.xlsx
+++ b/IJR-VI/exp_results/VIpercentage.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ammarbahman/Desktop/Eclipse workspace/Trunk/IJR-VI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ammarbahman/Desktop/Trunk/IJR-VI/exp_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C5562D-7EEE-644F-9E3E-CE3F447FD299}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1060" windowWidth="28720" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="17020" yWindow="5440" windowWidth="28720" windowHeight="17620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Test</t>
   </si>
@@ -54,12 +56,42 @@
   </si>
   <si>
     <t>Tdis_0K</t>
+  </si>
+  <si>
+    <t>eta_v</t>
+  </si>
+  <si>
+    <t>eta_c</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>eta_v_7K</t>
+  </si>
+  <si>
+    <t>eta_v_0K</t>
+  </si>
+  <si>
+    <t>eta_c_7K</t>
+  </si>
+  <si>
+    <t>eta_c_0K</t>
+  </si>
+  <si>
+    <t>no injection</t>
+  </si>
+  <si>
+    <t>7K superheat</t>
+  </si>
+  <si>
+    <t>0K (saturation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -89,8 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -100,6 +135,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -367,16 +405,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,8 +436,20 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -421,8 +471,20 @@
       <c r="G2">
         <v>0.56389999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>-2.480192903892521</v>
+      </c>
+      <c r="I2">
+        <v>-2.470145591362678</v>
+      </c>
+      <c r="J2">
+        <v>-2.8361465150993208</v>
+      </c>
+      <c r="K2">
+        <v>-5.9381645673155612</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -444,8 +506,20 @@
       <c r="G3">
         <v>-2.2949999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>-2.4436936936936959</v>
+      </c>
+      <c r="I3">
+        <v>-3.0940788440395774</v>
+      </c>
+      <c r="J3">
+        <v>-1.8918918918918837</v>
+      </c>
+      <c r="K3">
+        <v>-4.4604994502905653</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -467,8 +541,20 @@
       <c r="G4">
         <v>1.837</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>-2.0592445765884864</v>
+      </c>
+      <c r="I4">
+        <v>-3.4529349947455295</v>
+      </c>
+      <c r="J4">
+        <v>-1.8610285210879836</v>
+      </c>
+      <c r="K4">
+        <v>-4.9241855577240674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -490,8 +576,20 @@
       <c r="G5">
         <v>-0.99160000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>-1.667930250189529</v>
+      </c>
+      <c r="I5">
+        <v>-3.707518022657049</v>
+      </c>
+      <c r="J5">
+        <v>-1.1047330228528063</v>
+      </c>
+      <c r="K5">
+        <v>-4.5902604090039789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -513,8 +611,20 @@
       <c r="G6">
         <v>-1.1120000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>-1.4917421417154944</v>
+      </c>
+      <c r="I6">
+        <v>-3.0650784427658331</v>
+      </c>
+      <c r="J6">
+        <v>-1.0335641981885977</v>
+      </c>
+      <c r="K6">
+        <v>-3.8495061011040175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -536,8 +646,20 @@
       <c r="G7">
         <v>-1.3680000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>-1.2336488354780353</v>
+      </c>
+      <c r="I7">
+        <v>-2.5391758560650026</v>
+      </c>
+      <c r="J7">
+        <v>-0.58491970647665337</v>
+      </c>
+      <c r="K7">
+        <v>-2.9019152640742889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -559,8 +681,20 @@
       <c r="G8">
         <v>-4.9580000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>-1.2857294655190667</v>
+      </c>
+      <c r="I8">
+        <v>-3.4604623766750024</v>
+      </c>
+      <c r="J8">
+        <v>-1.2113484220592929</v>
+      </c>
+      <c r="K8">
+        <v>-5.4042114563392749</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -581,6 +715,414 @@
       </c>
       <c r="G9">
         <v>-4.109</v>
+      </c>
+      <c r="H9">
+        <v>-1.78362883533283</v>
+      </c>
+      <c r="I9">
+        <v>-4.1021897810219015</v>
+      </c>
+      <c r="J9">
+        <v>-0.7750291963053445</v>
+      </c>
+      <c r="K9">
+        <v>-3.9270072992700698</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2A5DD9-3BD5-6449-B5F2-6156F411E730}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>87.09</v>
+      </c>
+      <c r="C3" s="1">
+        <v>61.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>88.8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>63.67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>90.81</v>
+      </c>
+      <c r="C5" s="1">
+        <v>66.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>92.33</v>
+      </c>
+      <c r="C6" s="1">
+        <v>67.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>93.85</v>
+      </c>
+      <c r="C7" s="1">
+        <v>68.84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>94.03</v>
+      </c>
+      <c r="C8" s="1">
+        <v>68.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>94.11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>67.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>94.19</v>
+      </c>
+      <c r="C10" s="1">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>84.93</v>
+      </c>
+      <c r="C18" s="1">
+        <v>59.62</v>
+      </c>
+      <c r="D18">
+        <f>(B18-B3)/B3*100</f>
+        <v>-2.480192903892521</v>
+      </c>
+      <c r="E18">
+        <f>(C18-C3)/C3*100</f>
+        <v>-2.470145591362678</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>86.63</v>
+      </c>
+      <c r="C19" s="1">
+        <v>61.7</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D25" si="0">(B19-B4)/B4*100</f>
+        <v>-2.4436936936936959</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E25" si="1">(C19-C4)/C4*100</f>
+        <v>-3.0940788440395774</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1">
+        <v>88.94</v>
+      </c>
+      <c r="C20" s="1">
+        <v>64.31</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-2.0592445765884864</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>-3.4529349947455295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1">
+        <v>90.79</v>
+      </c>
+      <c r="C21" s="1">
+        <v>65.45</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-1.667930250189529</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>-3.707518022657049</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>92.45</v>
+      </c>
+      <c r="C22" s="1">
+        <v>66.73</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-1.4917421417154944</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>-3.0650784427658331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>92.87</v>
+      </c>
+      <c r="C23" s="1">
+        <v>67.17</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-1.2336488354780353</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>-2.5391758560650026</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>92.9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>65.56</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-1.2857294655190667</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>-3.4604623766750024</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>92.51</v>
+      </c>
+      <c r="C25" s="1">
+        <v>65.69</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-1.78362883533283</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>-4.1021897810219015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1">
+        <v>84.62</v>
+      </c>
+      <c r="C33" s="1">
+        <v>57.5</v>
+      </c>
+      <c r="D33">
+        <f>(B33-B3)/B3*100</f>
+        <v>-2.8361465150993208</v>
+      </c>
+      <c r="E33">
+        <f>(C33-C3)/C3*100</f>
+        <v>-5.9381645673155612</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="1">
+        <v>87.12</v>
+      </c>
+      <c r="C34" s="1">
+        <v>60.83</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:E34" si="2">(B34-B4)/B4*100</f>
+        <v>-1.8918918918918837</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>-4.4604994502905653</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="1">
+        <v>89.12</v>
+      </c>
+      <c r="C35" s="1">
+        <v>63.33</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:E35" si="3">(B35-B5)/B5*100</f>
+        <v>-1.8610285210879836</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>-4.9241855577240674</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="1">
+        <v>91.31</v>
+      </c>
+      <c r="C36" s="1">
+        <v>64.849999999999994</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ref="D36:E36" si="4">(B36-B6)/B6*100</f>
+        <v>-1.1047330228528063</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>-4.5902604090039789</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1">
+        <v>92.88</v>
+      </c>
+      <c r="C37" s="1">
+        <v>66.19</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:E37" si="5">(B37-B7)/B7*100</f>
+        <v>-1.0335641981885977</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="5"/>
+        <v>-3.8495061011040175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1">
+        <v>93.48</v>
+      </c>
+      <c r="C38" s="1">
+        <v>66.92</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:E38" si="6">(B38-B8)/B8*100</f>
+        <v>-0.58491970647665337</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="6"/>
+        <v>-2.9019152640742889</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1">
+        <v>92.97</v>
+      </c>
+      <c r="C39" s="1">
+        <v>64.239999999999995</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:E39" si="7">(B39-B9)/B9*100</f>
+        <v>-1.2113484220592929</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="7"/>
+        <v>-5.4042114563392749</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1">
+        <v>93.46</v>
+      </c>
+      <c r="C40" s="1">
+        <v>65.81</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:E40" si="8">(B40-B10)/B10*100</f>
+        <v>-0.7750291963053445</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="8"/>
+        <v>-3.9270072992700698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>